<commit_message>
fixed bug in the fedrollover
</commit_message>
<xml_diff>
--- a/.idea/auction_dates.xlsx
+++ b/.idea/auction_dates.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F621"/>
+  <dimension ref="A1:F635"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13640,10 +13640,8 @@
       <c r="A618" t="n">
         <v>0</v>
       </c>
-      <c r="B618" t="inlineStr">
-        <is>
-          <t>20082200</t>
-        </is>
+      <c r="B618" t="n">
+        <v>20082200</v>
       </c>
       <c r="C618" t="n">
         <v>0</v>
@@ -13662,10 +13660,8 @@
       <c r="A619" t="n">
         <v>0</v>
       </c>
-      <c r="B619" t="inlineStr">
-        <is>
-          <t>20082300</t>
-        </is>
+      <c r="B619" t="n">
+        <v>20082300</v>
       </c>
       <c r="C619" t="n">
         <v>0</v>
@@ -13686,26 +13682,20 @@
           <t>9127963B3</t>
         </is>
       </c>
-      <c r="B620" t="inlineStr">
-        <is>
-          <t>20082400</t>
-        </is>
+      <c r="B620" t="n">
+        <v>20082400</v>
       </c>
       <c r="C620" t="n">
         <v>105000000000</v>
       </c>
-      <c r="D620" t="inlineStr">
-        <is>
-          <t>54000000000</t>
-        </is>
+      <c r="D620" t="n">
+        <v>54000000000</v>
       </c>
       <c r="E620" t="n">
         <v>0.5142857142857142</v>
       </c>
-      <c r="F620" t="inlineStr">
-        <is>
-          <t>20082700</t>
-        </is>
+      <c r="F620" t="n">
+        <v>20082700</v>
       </c>
     </row>
     <row r="621">
@@ -13714,26 +13704,370 @@
           <t>912796XE4</t>
         </is>
       </c>
-      <c r="B621" t="inlineStr">
-        <is>
-          <t>20082400</t>
-        </is>
+      <c r="B621" t="n">
+        <v>20082400</v>
       </c>
       <c r="C621" t="n">
         <v>105000000000</v>
       </c>
-      <c r="D621" t="inlineStr">
-        <is>
-          <t>51000000000</t>
-        </is>
+      <c r="D621" t="n">
+        <v>51000000000</v>
       </c>
       <c r="E621" t="n">
         <v>0.4857142857142857</v>
       </c>
-      <c r="F621" t="inlineStr">
+      <c r="F621" t="n">
+        <v>20082700</v>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>91282CAG6</t>
+        </is>
+      </c>
+      <c r="B622" t="n">
+        <v>20082500</v>
+      </c>
+      <c r="C622" t="n">
+        <v>110000000000</v>
+      </c>
+      <c r="D622" t="n">
+        <v>50000000000</v>
+      </c>
+      <c r="E622" t="n">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="F622" t="n">
+        <v>20083100</v>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>912796TN9</t>
+        </is>
+      </c>
+      <c r="B623" t="n">
+        <v>20082500</v>
+      </c>
+      <c r="C623" t="n">
+        <v>110000000000</v>
+      </c>
+      <c r="D623" t="n">
+        <v>30000000000</v>
+      </c>
+      <c r="E623" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="F623" t="n">
+        <v>20082700</v>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>9127963L1</t>
+        </is>
+      </c>
+      <c r="B624" t="n">
+        <v>20082500</v>
+      </c>
+      <c r="C624" t="n">
+        <v>110000000000</v>
+      </c>
+      <c r="D624" t="n">
+        <v>30000000000</v>
+      </c>
+      <c r="E624" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="F624" t="n">
+        <v>20082700</v>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>9127965C9</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>20082600</t>
+        </is>
+      </c>
+      <c r="C625" t="n">
+        <v>128000000000</v>
+      </c>
+      <c r="D625" t="inlineStr">
+        <is>
+          <t>25000000000</t>
+        </is>
+      </c>
+      <c r="E625" t="n">
+        <v>0.1953125</v>
+      </c>
+      <c r="F625" t="inlineStr">
+        <is>
+          <t>20090100</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>912796B65</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>20082600</t>
+        </is>
+      </c>
+      <c r="C626" t="n">
+        <v>128000000000</v>
+      </c>
+      <c r="D626" t="inlineStr">
+        <is>
+          <t>30000000000</t>
+        </is>
+      </c>
+      <c r="E626" t="n">
+        <v>0.234375</v>
+      </c>
+      <c r="F626" t="inlineStr">
+        <is>
+          <t>20090100</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>91282CAJ0</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>20082600</t>
+        </is>
+      </c>
+      <c r="C627" t="n">
+        <v>128000000000</v>
+      </c>
+      <c r="D627" t="inlineStr">
+        <is>
+          <t>51000000000</t>
+        </is>
+      </c>
+      <c r="E627" t="n">
+        <v>0.3984375</v>
+      </c>
+      <c r="F627" t="inlineStr">
+        <is>
+          <t>20083100</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>91282CAA9</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>20082600</t>
+        </is>
+      </c>
+      <c r="C628" t="n">
+        <v>128000000000</v>
+      </c>
+      <c r="D628" t="inlineStr">
+        <is>
+          <t>22000000000</t>
+        </is>
+      </c>
+      <c r="E628" t="n">
+        <v>0.171875</v>
+      </c>
+      <c r="F628" t="inlineStr">
+        <is>
+          <t>20082800</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>9127964A4</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
         <is>
           <t>20082700</t>
         </is>
+      </c>
+      <c r="C629" t="n">
+        <v>112000000000</v>
+      </c>
+      <c r="D629" t="inlineStr">
+        <is>
+          <t>30000000000</t>
+        </is>
+      </c>
+      <c r="E629" t="n">
+        <v>0.2678571428571428</v>
+      </c>
+      <c r="F629" t="inlineStr">
+        <is>
+          <t>20090100</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>9127964K2</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>20082700</t>
+        </is>
+      </c>
+      <c r="C630" t="n">
+        <v>112000000000</v>
+      </c>
+      <c r="D630" t="inlineStr">
+        <is>
+          <t>35000000000</t>
+        </is>
+      </c>
+      <c r="E630" t="n">
+        <v>0.3125</v>
+      </c>
+      <c r="F630" t="inlineStr">
+        <is>
+          <t>20090100</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>91282CAH4</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>20082700</t>
+        </is>
+      </c>
+      <c r="C631" t="n">
+        <v>112000000000</v>
+      </c>
+      <c r="D631" t="inlineStr">
+        <is>
+          <t>47000000000</t>
+        </is>
+      </c>
+      <c r="E631" t="n">
+        <v>0.4196428571428572</v>
+      </c>
+      <c r="F631" t="inlineStr">
+        <is>
+          <t>20083100</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="n">
+        <v>0</v>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>20082800</t>
+        </is>
+      </c>
+      <c r="C632" t="n">
+        <v>0</v>
+      </c>
+      <c r="D632" t="n">
+        <v>0</v>
+      </c>
+      <c r="E632" t="n">
+        <v>0</v>
+      </c>
+      <c r="F632" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="n">
+        <v>0</v>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>20082900</t>
+        </is>
+      </c>
+      <c r="C633" t="n">
+        <v>0</v>
+      </c>
+      <c r="D633" t="n">
+        <v>0</v>
+      </c>
+      <c r="E633" t="n">
+        <v>0</v>
+      </c>
+      <c r="F633" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="n">
+        <v>0</v>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>20083000</t>
+        </is>
+      </c>
+      <c r="C634" t="n">
+        <v>0</v>
+      </c>
+      <c r="D634" t="n">
+        <v>0</v>
+      </c>
+      <c r="E634" t="n">
+        <v>0</v>
+      </c>
+      <c r="F634" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="n">
+        <v>0</v>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>20083100</t>
+        </is>
+      </c>
+      <c r="C635" t="n">
+        <v>0</v>
+      </c>
+      <c r="D635" t="n">
+        <v>0</v>
+      </c>
+      <c r="E635" t="n">
+        <v>0</v>
+      </c>
+      <c r="F635" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>